<commit_message>
Signed-off-by: Jigar Mehta Git <jigar.digital@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/java/com/assure/qa/testdata/AssureTestData.xlsx
+++ b/src/main/java/com/assure/qa/testdata/AssureTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>InputUsername</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>LoginTest</t>
+  </si>
+  <si>
+    <t>N0rthg4t311</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -374,11 +377,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -387,20 +388,31 @@
     <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -419,20 +431,9 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>